<commit_message>
new_morning_CSV + TAZ (- 18,19)
</commit_message>
<xml_diff>
--- a/out_in/xls/morning_in.xlsx
+++ b/out_in/xls/morning_in.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ACB76F-4C8C-4B23-A3DE-22E954BBE6C0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF607D2A-E9F9-4F5C-992E-D24081276E71}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -333,10 +333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,31 +855,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>0.33553333333333335</v>
+        <v>0.87360000000000004</v>
       </c>
       <c r="C17" s="1">
-        <v>1.6776666666666669</v>
+        <v>4.3680000000000003</v>
       </c>
       <c r="D17" s="1">
-        <v>1.6776666666666669</v>
+        <v>4.3680000000000003</v>
       </c>
       <c r="E17" s="1">
-        <v>5.0330000000000004</v>
+        <v>13.103999999999999</v>
       </c>
       <c r="F17" s="1">
-        <v>1.5099</v>
+        <v>3.9312</v>
       </c>
       <c r="G17" s="1">
-        <v>2.6842666666666668</v>
+        <v>6.9888000000000003</v>
       </c>
       <c r="H17" s="1">
-        <v>1.6776666666666669</v>
+        <v>4.3680000000000003</v>
       </c>
       <c r="I17" s="1">
-        <v>0.50329999999999997</v>
+        <v>1.3104</v>
       </c>
       <c r="J17" s="1">
-        <v>1.6776666666666669</v>
+        <v>4.3680000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -887,1247 +887,1183 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>0.28606666666666664</v>
+        <v>0.9355500000000001</v>
       </c>
       <c r="C18" s="1">
-        <v>1.4303333333333335</v>
+        <v>4.6777500000000005</v>
       </c>
       <c r="D18" s="1">
-        <v>1.4303333333333335</v>
+        <v>4.6777500000000005</v>
       </c>
       <c r="E18" s="1">
-        <v>4.2909999999999995</v>
+        <v>14.033250000000001</v>
       </c>
       <c r="F18" s="1">
-        <v>1.2872999999999999</v>
+        <v>4.209975</v>
       </c>
       <c r="G18" s="1">
-        <v>2.2885333333333331</v>
+        <v>7.4844000000000008</v>
       </c>
       <c r="H18" s="1">
-        <v>1.4303333333333335</v>
+        <v>4.6777500000000005</v>
       </c>
       <c r="I18" s="1">
-        <v>0.42909999999999998</v>
+        <v>1.4033250000000002</v>
       </c>
       <c r="J18" s="1">
-        <v>1.4303333333333335</v>
+        <v>4.6777500000000005</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>0.51800000000000002</v>
+        <v>0.42886666666666673</v>
       </c>
       <c r="C19" s="1">
-        <v>2.59</v>
+        <v>2.1443333333333334</v>
       </c>
       <c r="D19" s="1">
-        <v>2.59</v>
+        <v>2.1443333333333334</v>
       </c>
       <c r="E19" s="1">
-        <v>7.77</v>
+        <v>6.4330000000000007</v>
       </c>
       <c r="F19" s="1">
-        <v>2.331</v>
+        <v>1.9299000000000002</v>
       </c>
       <c r="G19" s="1">
-        <v>4.1440000000000001</v>
+        <v>3.4309333333333338</v>
       </c>
       <c r="H19" s="1">
-        <v>2.59</v>
+        <v>2.1443333333333334</v>
       </c>
       <c r="I19" s="1">
-        <v>0.77699999999999991</v>
+        <v>0.64329999999999998</v>
       </c>
       <c r="J19" s="1">
-        <v>2.59</v>
+        <v>2.1443333333333334</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>0.56793333333333329</v>
+        <v>1.2606999999999999</v>
       </c>
       <c r="C20" s="1">
-        <v>2.8396666666666661</v>
+        <v>6.3034999999999997</v>
       </c>
       <c r="D20" s="1">
-        <v>2.8396666666666661</v>
+        <v>6.3034999999999997</v>
       </c>
       <c r="E20" s="1">
-        <v>8.5189999999999984</v>
+        <v>18.910499999999999</v>
       </c>
       <c r="F20" s="1">
-        <v>2.5556999999999994</v>
+        <v>5.6731499999999997</v>
       </c>
       <c r="G20" s="1">
-        <v>4.5434666666666663</v>
+        <v>10.085599999999999</v>
       </c>
       <c r="H20" s="1">
-        <v>2.8396666666666661</v>
+        <v>6.3034999999999997</v>
       </c>
       <c r="I20" s="1">
-        <v>0.85189999999999977</v>
+        <v>1.8910499999999999</v>
       </c>
       <c r="J20" s="1">
-        <v>2.8396666666666661</v>
+        <v>6.3034999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>0.42886666666666673</v>
+        <v>0.85119999999999996</v>
       </c>
       <c r="C21" s="1">
-        <v>2.1443333333333334</v>
+        <v>4.2559999999999993</v>
       </c>
       <c r="D21" s="1">
-        <v>2.1443333333333334</v>
+        <v>4.2559999999999993</v>
       </c>
       <c r="E21" s="1">
-        <v>6.4330000000000007</v>
+        <v>12.767999999999999</v>
       </c>
       <c r="F21" s="1">
-        <v>1.9299000000000002</v>
+        <v>3.8303999999999996</v>
       </c>
       <c r="G21" s="1">
-        <v>3.4309333333333338</v>
+        <v>6.8095999999999997</v>
       </c>
       <c r="H21" s="1">
-        <v>2.1443333333333334</v>
+        <v>4.2559999999999993</v>
       </c>
       <c r="I21" s="1">
-        <v>0.64329999999999998</v>
+        <v>1.2767999999999997</v>
       </c>
       <c r="J21" s="1">
-        <v>2.1443333333333334</v>
+        <v>4.2559999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>1.2606999999999999</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>6.3034999999999997</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>6.3034999999999997</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>18.910499999999999</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>5.6731499999999997</v>
+        <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>10.085599999999999</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>6.3034999999999997</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1">
-        <v>1.8910499999999999</v>
+        <v>0</v>
       </c>
       <c r="J22" s="1">
-        <v>6.3034999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>0.85119999999999996</v>
+        <v>0.59966666666666668</v>
       </c>
       <c r="C23" s="1">
-        <v>4.2559999999999993</v>
+        <v>2.9983333333333335</v>
       </c>
       <c r="D23" s="1">
-        <v>4.2559999999999993</v>
+        <v>2.9983333333333335</v>
       </c>
       <c r="E23" s="1">
-        <v>12.767999999999999</v>
+        <v>8.9949999999999992</v>
       </c>
       <c r="F23" s="1">
-        <v>3.8303999999999996</v>
+        <v>2.6985000000000001</v>
       </c>
       <c r="G23" s="1">
-        <v>6.8095999999999997</v>
+        <v>4.7973333333333334</v>
       </c>
       <c r="H23" s="1">
-        <v>4.2559999999999993</v>
+        <v>2.9983333333333335</v>
       </c>
       <c r="I23" s="1">
-        <v>1.2767999999999997</v>
+        <v>0.89949999999999997</v>
       </c>
       <c r="J23" s="1">
-        <v>4.2559999999999993</v>
+        <v>2.9983333333333335</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>3.1500000000000004</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>3.1500000000000004</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>2.835</v>
       </c>
       <c r="G24" s="1">
-        <v>0</v>
+        <v>5.04</v>
       </c>
       <c r="H24" s="1">
-        <v>0</v>
+        <v>3.1500000000000004</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
+        <v>3.1500000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>0.59966666666666668</v>
+        <v>0.504</v>
       </c>
       <c r="C25" s="1">
-        <v>2.9983333333333335</v>
+        <v>2.52</v>
       </c>
       <c r="D25" s="1">
-        <v>2.9983333333333335</v>
+        <v>2.52</v>
       </c>
       <c r="E25" s="1">
-        <v>8.9949999999999992</v>
+        <v>7.56</v>
       </c>
       <c r="F25" s="1">
-        <v>2.6985000000000001</v>
+        <v>2.2679999999999998</v>
       </c>
       <c r="G25" s="1">
-        <v>4.7973333333333334</v>
+        <v>4.032</v>
       </c>
       <c r="H25" s="1">
-        <v>2.9983333333333335</v>
+        <v>2.52</v>
       </c>
       <c r="I25" s="1">
-        <v>0.89949999999999997</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="J25" s="1">
-        <v>2.9983333333333335</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1">
-        <v>0.49</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="C26" s="1">
-        <v>2.4500000000000002</v>
+        <v>1.75</v>
       </c>
       <c r="D26" s="1">
-        <v>2.4500000000000002</v>
+        <v>1.75</v>
       </c>
       <c r="E26" s="1">
-        <v>7.35</v>
+        <v>5.25</v>
       </c>
       <c r="F26" s="1">
-        <v>2.2050000000000001</v>
+        <v>1.575</v>
       </c>
       <c r="G26" s="1">
-        <v>3.92</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="H26" s="1">
-        <v>2.4500000000000002</v>
+        <v>1.75</v>
       </c>
       <c r="I26" s="1">
-        <v>0.73499999999999999</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="J26" s="1">
-        <v>2.4500000000000002</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
-        <v>0.36399999999999999</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="C27" s="1">
-        <v>1.82</v>
+        <v>3.78</v>
       </c>
       <c r="D27" s="1">
-        <v>1.82</v>
+        <v>3.78</v>
       </c>
       <c r="E27" s="1">
-        <v>5.46</v>
+        <v>11.339999999999998</v>
       </c>
       <c r="F27" s="1">
-        <v>1.6379999999999999</v>
+        <v>3.4019999999999997</v>
       </c>
       <c r="G27" s="1">
-        <v>2.9119999999999999</v>
+        <v>6.048</v>
       </c>
       <c r="H27" s="1">
-        <v>1.82</v>
+        <v>3.78</v>
       </c>
       <c r="I27" s="1">
-        <v>0.54599999999999993</v>
+        <v>1.1339999999999999</v>
       </c>
       <c r="J27" s="1">
-        <v>1.82</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1">
-        <v>0.21</v>
+        <v>0.42</v>
       </c>
       <c r="C28" s="1">
-        <v>1.05</v>
+        <v>2.1</v>
       </c>
       <c r="D28" s="1">
-        <v>1.05</v>
+        <v>2.1</v>
       </c>
       <c r="E28" s="1">
-        <v>3.15</v>
+        <v>6.3</v>
       </c>
       <c r="F28" s="1">
-        <v>0.94499999999999995</v>
+        <v>1.89</v>
       </c>
       <c r="G28" s="1">
-        <v>1.68</v>
+        <v>3.36</v>
       </c>
       <c r="H28" s="1">
-        <v>1.05</v>
+        <v>2.1</v>
       </c>
       <c r="I28" s="1">
-        <v>0.315</v>
+        <v>0.63</v>
       </c>
       <c r="J28" s="1">
-        <v>1.05</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1">
-        <v>0.61599999999999999</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="C29" s="1">
-        <v>3.08</v>
+        <v>2.31</v>
       </c>
       <c r="D29" s="1">
-        <v>3.08</v>
+        <v>2.31</v>
       </c>
       <c r="E29" s="1">
-        <v>9.24</v>
+        <v>6.9300000000000006</v>
       </c>
       <c r="F29" s="1">
-        <v>2.7719999999999998</v>
+        <v>2.0790000000000002</v>
       </c>
       <c r="G29" s="1">
-        <v>4.9279999999999999</v>
+        <v>3.6960000000000002</v>
       </c>
       <c r="H29" s="1">
-        <v>3.08</v>
+        <v>2.31</v>
       </c>
       <c r="I29" s="1">
-        <v>0.92399999999999993</v>
+        <v>0.69300000000000006</v>
       </c>
       <c r="J29" s="1">
-        <v>3.08</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="C30" s="1">
-        <v>1.4000000000000001</v>
+        <v>2.7300000000000004</v>
       </c>
       <c r="D30" s="1">
-        <v>1.4000000000000001</v>
+        <v>2.7300000000000004</v>
       </c>
       <c r="E30" s="1">
-        <v>4.2</v>
+        <v>8.19</v>
       </c>
       <c r="F30" s="1">
-        <v>1.26</v>
+        <v>2.4569999999999999</v>
       </c>
       <c r="G30" s="1">
-        <v>2.2400000000000002</v>
+        <v>4.3680000000000003</v>
       </c>
       <c r="H30" s="1">
-        <v>1.4000000000000001</v>
+        <v>2.7300000000000004</v>
       </c>
       <c r="I30" s="1">
-        <v>0.42</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="J30" s="1">
-        <v>1.4000000000000001</v>
+        <v>2.7300000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1">
-        <v>0.32200000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="C31" s="1">
-        <v>1.6100000000000003</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D31" s="1">
-        <v>1.6100000000000003</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="E31" s="1">
-        <v>4.83</v>
+        <v>7.35</v>
       </c>
       <c r="F31" s="1">
-        <v>1.4490000000000001</v>
+        <v>2.2050000000000001</v>
       </c>
       <c r="G31" s="1">
-        <v>2.5760000000000001</v>
+        <v>3.92</v>
       </c>
       <c r="H31" s="1">
-        <v>1.6100000000000003</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="I31" s="1">
-        <v>0.48300000000000004</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="J31" s="1">
-        <v>1.6100000000000003</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1">
-        <v>0.40600000000000003</v>
+        <v>18.666666666666664</v>
       </c>
       <c r="C32" s="1">
-        <v>2.0300000000000002</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="D32" s="1">
-        <v>2.0300000000000002</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="E32" s="1">
-        <v>6.09</v>
+        <v>279.99999999999994</v>
       </c>
       <c r="F32" s="1">
-        <v>1.827</v>
+        <v>83.999999999999986</v>
       </c>
       <c r="G32" s="1">
-        <v>3.2480000000000002</v>
+        <v>149.33333333333331</v>
       </c>
       <c r="H32" s="1">
-        <v>2.0300000000000002</v>
+        <v>93.333333333333329</v>
       </c>
       <c r="I32" s="1">
-        <v>0.60899999999999999</v>
+        <v>27.999999999999996</v>
       </c>
       <c r="J32" s="1">
-        <v>2.0300000000000002</v>
+        <v>93.333333333333329</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1">
-        <v>0.35000000000000003</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="C33" s="1">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="D33" s="1">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="E33" s="1">
-        <v>5.25</v>
+        <v>5.7749999999999995</v>
       </c>
       <c r="F33" s="1">
-        <v>1.575</v>
+        <v>1.7324999999999999</v>
       </c>
       <c r="G33" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.08</v>
       </c>
       <c r="H33" s="1">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="I33" s="1">
-        <v>0.52500000000000002</v>
+        <v>0.57750000000000001</v>
       </c>
       <c r="J33" s="1">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1">
-        <v>18.666666666666664</v>
+        <v>0.504</v>
       </c>
       <c r="C34" s="1">
-        <v>93.333333333333329</v>
+        <v>2.52</v>
       </c>
       <c r="D34" s="1">
-        <v>93.333333333333329</v>
+        <v>2.52</v>
       </c>
       <c r="E34" s="1">
-        <v>279.99999999999994</v>
+        <v>7.56</v>
       </c>
       <c r="F34" s="1">
-        <v>83.999999999999986</v>
+        <v>2.2679999999999998</v>
       </c>
       <c r="G34" s="1">
-        <v>149.33333333333331</v>
+        <v>4.032</v>
       </c>
       <c r="H34" s="1">
-        <v>93.333333333333329</v>
+        <v>2.52</v>
       </c>
       <c r="I34" s="1">
-        <v>27.999999999999996</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="J34" s="1">
-        <v>93.333333333333329</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1">
-        <v>0.245</v>
+        <v>0.63</v>
       </c>
       <c r="C35" s="1">
-        <v>1.2250000000000001</v>
+        <v>3.1500000000000004</v>
       </c>
       <c r="D35" s="1">
-        <v>1.2250000000000001</v>
+        <v>3.1500000000000004</v>
       </c>
       <c r="E35" s="1">
-        <v>3.6749999999999998</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="F35" s="1">
-        <v>1.1025</v>
+        <v>2.835</v>
       </c>
       <c r="G35" s="1">
-        <v>1.96</v>
+        <v>5.04</v>
       </c>
       <c r="H35" s="1">
-        <v>1.2250000000000001</v>
+        <v>3.1500000000000004</v>
       </c>
       <c r="I35" s="1">
-        <v>0.36749999999999999</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="J35" s="1">
-        <v>1.2250000000000001</v>
+        <v>3.1500000000000004</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1">
-        <v>0.36399999999999999</v>
+        <v>0.62439999999999996</v>
       </c>
       <c r="C36" s="1">
-        <v>1.82</v>
+        <v>3.1219999999999999</v>
       </c>
       <c r="D36" s="1">
-        <v>1.82</v>
+        <v>3.1219999999999999</v>
       </c>
       <c r="E36" s="1">
-        <v>5.46</v>
+        <v>9.3659999999999997</v>
       </c>
       <c r="F36" s="1">
-        <v>1.6379999999999999</v>
+        <v>2.8097999999999996</v>
       </c>
       <c r="G36" s="1">
-        <v>2.9119999999999999</v>
+        <v>4.9951999999999996</v>
       </c>
       <c r="H36" s="1">
-        <v>1.82</v>
+        <v>3.1219999999999999</v>
       </c>
       <c r="I36" s="1">
-        <v>0.54599999999999993</v>
+        <v>0.93659999999999988</v>
       </c>
       <c r="J36" s="1">
-        <v>1.82</v>
+        <v>3.1219999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1">
-        <v>0.49</v>
+        <v>0.59360000000000002</v>
       </c>
       <c r="C37" s="1">
-        <v>2.4500000000000002</v>
+        <v>2.968</v>
       </c>
       <c r="D37" s="1">
-        <v>2.4500000000000002</v>
+        <v>2.968</v>
       </c>
       <c r="E37" s="1">
-        <v>7.35</v>
+        <v>8.9039999999999999</v>
       </c>
       <c r="F37" s="1">
-        <v>2.2050000000000001</v>
+        <v>2.6711999999999998</v>
       </c>
       <c r="G37" s="1">
-        <v>3.92</v>
+        <v>4.7488000000000001</v>
       </c>
       <c r="H37" s="1">
-        <v>2.4500000000000002</v>
+        <v>2.968</v>
       </c>
       <c r="I37" s="1">
-        <v>0.73499999999999999</v>
+        <v>0.89039999999999997</v>
       </c>
       <c r="J37" s="1">
-        <v>2.4500000000000002</v>
+        <v>2.968</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1">
-        <v>0.4844</v>
+        <v>0.55159999999999998</v>
       </c>
       <c r="C38" s="1">
-        <v>2.4220000000000002</v>
+        <v>2.758</v>
       </c>
       <c r="D38" s="1">
-        <v>2.4220000000000002</v>
+        <v>2.758</v>
       </c>
       <c r="E38" s="1">
-        <v>7.2659999999999991</v>
+        <v>8.2739999999999991</v>
       </c>
       <c r="F38" s="1">
-        <v>2.1797999999999997</v>
+        <v>2.4821999999999997</v>
       </c>
       <c r="G38" s="1">
-        <v>3.8752</v>
+        <v>4.4127999999999998</v>
       </c>
       <c r="H38" s="1">
-        <v>2.4220000000000002</v>
+        <v>2.758</v>
       </c>
       <c r="I38" s="1">
-        <v>0.72659999999999991</v>
+        <v>0.82739999999999991</v>
       </c>
       <c r="J38" s="1">
-        <v>2.4220000000000002</v>
+        <v>2.758</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1">
-        <v>0.4536</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="C39" s="1">
-        <v>2.2680000000000002</v>
+        <v>1.9600000000000002</v>
       </c>
       <c r="D39" s="1">
-        <v>2.2680000000000002</v>
+        <v>1.9600000000000002</v>
       </c>
       <c r="E39" s="1">
-        <v>6.8039999999999994</v>
+        <v>5.88</v>
       </c>
       <c r="F39" s="1">
-        <v>2.0411999999999999</v>
+        <v>1.764</v>
       </c>
       <c r="G39" s="1">
-        <v>3.6288</v>
+        <v>3.1360000000000001</v>
       </c>
       <c r="H39" s="1">
-        <v>2.2680000000000002</v>
+        <v>1.9600000000000002</v>
       </c>
       <c r="I39" s="1">
-        <v>0.6804</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="J39" s="1">
-        <v>2.2680000000000002</v>
+        <v>1.9600000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1">
-        <v>0.41159999999999997</v>
+        <v>1.54</v>
       </c>
       <c r="C40" s="1">
-        <v>2.0579999999999998</v>
+        <v>7.7</v>
       </c>
       <c r="D40" s="1">
-        <v>2.0579999999999998</v>
+        <v>7.7</v>
       </c>
       <c r="E40" s="1">
-        <v>6.1739999999999995</v>
+        <v>23.099999999999998</v>
       </c>
       <c r="F40" s="1">
-        <v>1.8521999999999998</v>
+        <v>6.93</v>
       </c>
       <c r="G40" s="1">
-        <v>3.2927999999999997</v>
+        <v>12.32</v>
       </c>
       <c r="H40" s="1">
-        <v>2.0579999999999998</v>
+        <v>7.7</v>
       </c>
       <c r="I40" s="1">
-        <v>0.61739999999999995</v>
+        <v>2.31</v>
       </c>
       <c r="J40" s="1">
-        <v>2.0579999999999998</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1">
-        <v>0.252</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C41" s="1">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="E41" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="F41" s="1">
         <v>1.26</v>
       </c>
-      <c r="D41" s="1">
-        <v>1.26</v>
-      </c>
-      <c r="E41" s="1">
-        <v>3.78</v>
-      </c>
-      <c r="F41" s="1">
-        <v>1.1339999999999999</v>
-      </c>
       <c r="G41" s="1">
-        <v>2.016</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="H41" s="1">
-        <v>1.26</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="I41" s="1">
-        <v>0.378</v>
+        <v>0.42</v>
       </c>
       <c r="J41" s="1">
-        <v>1.26</v>
+        <v>1.4000000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.84</v>
       </c>
       <c r="C42" s="1">
-        <v>1.4000000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="D42" s="1">
-        <v>1.4000000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="E42" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3.78</v>
+      </c>
+      <c r="G42" s="1">
+        <v>6.72</v>
+      </c>
+      <c r="H42" s="1">
         <v>4.2</v>
       </c>
-      <c r="F42" s="1">
+      <c r="I42" s="1">
         <v>1.26</v>
       </c>
-      <c r="G42" s="1">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="H42" s="1">
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="I42" s="1">
-        <v>0.42</v>
-      </c>
       <c r="J42" s="1">
-        <v>1.4000000000000001</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1">
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="C43" s="1">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="D43" s="1">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E43" s="1">
-        <v>0</v>
+        <v>12.6</v>
       </c>
       <c r="F43" s="1">
-        <v>0</v>
+        <v>3.78</v>
       </c>
       <c r="G43" s="1">
-        <v>0</v>
+        <v>6.72</v>
       </c>
       <c r="H43" s="1">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="I43" s="1">
-        <v>0</v>
+        <v>1.26</v>
       </c>
       <c r="J43" s="1">
-        <v>0</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1">
-        <v>0</v>
+        <v>7.2916666666666661</v>
       </c>
       <c r="C44" s="1">
-        <v>0</v>
+        <v>36.458333333333336</v>
       </c>
       <c r="D44" s="1">
-        <v>0</v>
+        <v>36.458333333333336</v>
       </c>
       <c r="E44" s="1">
-        <v>0</v>
+        <v>109.37499999999999</v>
       </c>
       <c r="F44" s="1">
-        <v>0</v>
+        <v>32.8125</v>
       </c>
       <c r="G44" s="1">
-        <v>0</v>
+        <v>58.333333333333329</v>
       </c>
       <c r="H44" s="1">
-        <v>0</v>
+        <v>36.458333333333336</v>
       </c>
       <c r="I44" s="1">
-        <v>0</v>
+        <v>10.937499999999998</v>
       </c>
       <c r="J44" s="1">
-        <v>0</v>
+        <v>36.458333333333336</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C45" s="1">
-        <v>0</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="D45" s="1">
-        <v>0</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="E45" s="1">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="F45" s="1">
-        <v>0</v>
+        <v>1.26</v>
       </c>
       <c r="G45" s="1">
-        <v>0</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="H45" s="1">
-        <v>0</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="I45" s="1">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="J45" s="1">
-        <v>0</v>
+        <v>1.4000000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1">
-        <v>7.2916666666666661</v>
+        <v>1.61</v>
       </c>
       <c r="C46" s="1">
-        <v>36.458333333333336</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="D46" s="1">
-        <v>36.458333333333336</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="E46" s="1">
-        <v>109.37499999999999</v>
+        <v>24.15</v>
       </c>
       <c r="F46" s="1">
-        <v>32.8125</v>
+        <v>7.2450000000000001</v>
       </c>
       <c r="G46" s="1">
-        <v>58.333333333333329</v>
+        <v>12.88</v>
       </c>
       <c r="H46" s="1">
-        <v>36.458333333333336</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="I46" s="1">
-        <v>10.937499999999998</v>
+        <v>2.415</v>
       </c>
       <c r="J46" s="1">
-        <v>36.458333333333336</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="C47" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="D47" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
+        <v>6.3</v>
       </c>
       <c r="F47" s="1">
-        <v>0</v>
+        <v>1.89</v>
       </c>
       <c r="G47" s="1">
-        <v>0</v>
+        <v>3.36</v>
       </c>
       <c r="H47" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="I47" s="1">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="J47" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1">
-        <v>1.47</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="C48" s="1">
-        <v>7.3500000000000005</v>
+        <v>3.5</v>
       </c>
       <c r="D48" s="1">
-        <v>7.3500000000000005</v>
+        <v>3.5</v>
       </c>
       <c r="E48" s="1">
-        <v>22.05</v>
+        <v>10.5</v>
       </c>
       <c r="F48" s="1">
-        <v>6.6149999999999993</v>
+        <v>3.15</v>
       </c>
       <c r="G48" s="1">
-        <v>11.76</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="H48" s="1">
-        <v>7.3500000000000005</v>
+        <v>3.5</v>
       </c>
       <c r="I48" s="1">
-        <v>2.2050000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="J48" s="1">
-        <v>7.3500000000000005</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1">
-        <v>0</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="C49" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="D49" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E49" s="1">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="F49" s="1">
-        <v>0</v>
+        <v>3.15</v>
       </c>
       <c r="G49" s="1">
-        <v>0</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="H49" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I49" s="1">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="J49" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="C50" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="D50" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="E50" s="1">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
       <c r="F50" s="1">
-        <v>2.52</v>
+        <v>3.15</v>
       </c>
       <c r="G50" s="1">
-        <v>4.4800000000000004</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="H50" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="I50" s="1">
-        <v>0.84</v>
+        <v>1.05</v>
       </c>
       <c r="J50" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="C51" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="D51" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="E51" s="1">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
       <c r="F51" s="1">
-        <v>2.52</v>
+        <v>3.15</v>
       </c>
       <c r="G51" s="1">
-        <v>4.4800000000000004</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="H51" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="I51" s="1">
-        <v>0.84</v>
+        <v>1.05</v>
       </c>
       <c r="J51" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="C52" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="D52" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="E52" s="1">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
       <c r="F52" s="1">
-        <v>2.52</v>
+        <v>3.15</v>
       </c>
       <c r="G52" s="1">
-        <v>4.4800000000000004</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="H52" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="I52" s="1">
-        <v>0.84</v>
+        <v>1.05</v>
       </c>
       <c r="J52" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="C53" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="D53" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="E53" s="1">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
       <c r="F53" s="1">
-        <v>2.52</v>
+        <v>3.15</v>
       </c>
       <c r="G53" s="1">
-        <v>4.4800000000000004</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="H53" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="I53" s="1">
-        <v>0.84</v>
+        <v>1.05</v>
       </c>
       <c r="J53" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B54" s="1">
-        <v>0.56000000000000005</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="C54" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="D54" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="E54" s="1">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
       <c r="F54" s="1">
-        <v>2.52</v>
+        <v>3.15</v>
       </c>
       <c r="G54" s="1">
-        <v>4.4800000000000004</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="H54" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
       <c r="I54" s="1">
-        <v>0.84</v>
+        <v>1.05</v>
       </c>
       <c r="J54" s="1">
-        <v>2.8000000000000003</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="C55" s="1">
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="D55" s="1">
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="E55" s="1">
-        <v>8.4</v>
-      </c>
-      <c r="F55" s="1">
-        <v>2.52</v>
-      </c>
-      <c r="G55" s="1">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="H55" s="1">
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="I55" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="J55" s="1">
-        <v>2.8000000000000003</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="C56" s="1">
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="D56" s="1">
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="E56" s="1">
-        <v>8.4</v>
-      </c>
-      <c r="F56" s="1">
-        <v>2.52</v>
-      </c>
-      <c r="G56" s="1">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="H56" s="1">
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="I56" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="J56" s="1">
-        <v>2.8000000000000003</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>